<commit_message>
add customer excel with updated ids
</commit_message>
<xml_diff>
--- a/data/AddCustomer.xlsx
+++ b/data/AddCustomer.xlsx
@@ -35,9 +35,6 @@
     <t>CustomerName</t>
   </si>
   <si>
-    <t>TC001_AddCustomer_Valid</t>
-  </si>
-  <si>
     <t>Add a customer by providing valid customerId and customerName</t>
   </si>
   <si>
@@ -47,15 +44,6 @@
     <t>C01</t>
   </si>
   <si>
-    <t>TC002_AddCustomer_CustomerId_Empty</t>
-  </si>
-  <si>
-    <t>TC003_AddCustomer_CustomerName_Empty</t>
-  </si>
-  <si>
-    <t>TC004_AddCustomer_Blank</t>
-  </si>
-  <si>
     <t>Add a customer by providing valid  customerName only</t>
   </si>
   <si>
@@ -75,6 +63,18 @@
   </si>
   <si>
     <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>TC009_AddCustomer_Valid</t>
+  </si>
+  <si>
+    <t>TC010_AddCustomer_CustomerId_Empty</t>
+  </si>
+  <si>
+    <t>TC011_AddCustomer_CustomerName_Empty</t>
+  </si>
+  <si>
+    <t>TC012_AddCustomer_Blank</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -412,7 +414,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -426,58 +428,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>